<commit_message>
Daily raw snapshot: 2025-08-22T12:25:48Z
</commit_message>
<xml_diff>
--- a/archive/2025-08/ETF_Investment_Portfolio_20250822.xlsx
+++ b/archive/2025-08/ETF_Investment_Portfolio_20250822.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="220">
-  <si>
-    <t xml:space="preserve">資料日期：114/08/21</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="221">
+  <si>
+    <t xml:space="preserve">資料日期：114/08/22</t>
   </si>
   <si>
     <t xml:space="preserve">基金資產</t>
@@ -23,7 +23,7 @@
     <t xml:space="preserve">淨資產</t>
   </si>
   <si>
-    <t xml:space="preserve">NTD 16,454,906,203</t>
+    <t xml:space="preserve">NTD 16,362,423,799</t>
   </si>
   <si>
     <t xml:space="preserve">流通在外單位數</t>
@@ -35,7 +35,7 @@
     <t xml:space="preserve">每單位淨值</t>
   </si>
   <si>
-    <t xml:space="preserve">NTD 12.71</t>
+    <t xml:space="preserve">NTD 12.64</t>
   </si>
   <si>
     <t xml:space="preserve">項目</t>
@@ -59,19 +59,19 @@
     <t xml:space="preserve">股票</t>
   </si>
   <si>
-    <t xml:space="preserve">NTD 15,439,488,834</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93.83%</t>
+    <t xml:space="preserve">NTD 15,582,415,453</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95.23%</t>
   </si>
   <si>
     <t xml:space="preserve">現金</t>
   </si>
   <si>
-    <t xml:space="preserve">NTD 982,578,508</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.97%</t>
+    <t xml:space="preserve">NTD 1,793,626,865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.96%</t>
   </si>
   <si>
     <t xml:space="preserve">期貨保證金</t>
@@ -89,10 +89,10 @@
     <t xml:space="preserve">應收付證券款</t>
   </si>
   <si>
-    <t xml:space="preserve">NTD -1,171,942,437</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-7.12%</t>
+    <t xml:space="preserve">NTD -1,471,641,936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8.99%</t>
   </si>
   <si>
     <t xml:space="preserve">股票代號</t>
@@ -113,10 +113,22 @@
     <t xml:space="preserve">台積電</t>
   </si>
   <si>
-    <t xml:space="preserve">1,287,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.99%</t>
+    <t xml:space="preserve">1,352,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.38%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">台達電</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,498,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.08%</t>
   </si>
   <si>
     <t xml:space="preserve">2383</t>
@@ -128,7 +140,7 @@
     <t xml:space="preserve">816,000</t>
   </si>
   <si>
-    <t xml:space="preserve">6.12%</t>
+    <t xml:space="preserve">6.01%</t>
   </si>
   <si>
     <t xml:space="preserve">3017</t>
@@ -140,7 +152,7 @@
     <t xml:space="preserve">946,000</t>
   </si>
   <si>
-    <t xml:space="preserve">6.04%</t>
+    <t xml:space="preserve">5.95%</t>
   </si>
   <si>
     <t xml:space="preserve">3665</t>
@@ -152,19 +164,7 @@
     <t xml:space="preserve">1,006,848</t>
   </si>
   <si>
-    <t xml:space="preserve">5.98%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">台達電</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,498,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.90%</t>
+    <t xml:space="preserve">5.80%</t>
   </si>
   <si>
     <t xml:space="preserve">2345</t>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">924,000</t>
   </si>
   <si>
-    <t xml:space="preserve">5.33%</t>
+    <t xml:space="preserve">5.31%</t>
   </si>
   <si>
     <t xml:space="preserve">3661</t>
@@ -188,7 +188,7 @@
     <t xml:space="preserve">223,000</t>
   </si>
   <si>
-    <t xml:space="preserve">5.13%</t>
+    <t xml:space="preserve">5.03%</t>
   </si>
   <si>
     <t xml:space="preserve">2368</t>
@@ -200,7 +200,7 @@
     <t xml:space="preserve">1,778,000</t>
   </si>
   <si>
-    <t xml:space="preserve">4.85%</t>
+    <t xml:space="preserve">4.99%</t>
   </si>
   <si>
     <t xml:space="preserve">2454</t>
@@ -212,7 +212,19 @@
     <t xml:space="preserve">560,000</t>
   </si>
   <si>
-    <t xml:space="preserve">4.65%</t>
+    <t xml:space="preserve">4.67%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3653</t>
+  </si>
+  <si>
+    <t xml:space="preserve">健策</t>
+  </si>
+  <si>
+    <t xml:space="preserve">352,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.51%</t>
   </si>
   <si>
     <t xml:space="preserve">2317</t>
@@ -224,19 +236,7 @@
     <t xml:space="preserve">2,734,000</t>
   </si>
   <si>
-    <t xml:space="preserve">3.42%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3653</t>
-  </si>
-  <si>
-    <t xml:space="preserve">健策</t>
-  </si>
-  <si>
-    <t xml:space="preserve">352,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.36%</t>
+    <t xml:space="preserve">3.38%</t>
   </si>
   <si>
     <t xml:space="preserve">4958</t>
@@ -245,10 +245,10 @@
     <t xml:space="preserve">臻鼎-KY</t>
   </si>
   <si>
-    <t xml:space="preserve">3,029,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.09%</t>
+    <t xml:space="preserve">3,198,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.34%</t>
   </si>
   <si>
     <t xml:space="preserve">8046</t>
@@ -260,7 +260,7 @@
     <t xml:space="preserve">2,820,000</t>
   </si>
   <si>
-    <t xml:space="preserve">2.90%</t>
+    <t xml:space="preserve">2.97%</t>
   </si>
   <si>
     <t xml:space="preserve">8210</t>
@@ -272,7 +272,7 @@
     <t xml:space="preserve">736,000</t>
   </si>
   <si>
-    <t xml:space="preserve">2.71%</t>
+    <t xml:space="preserve">2.69%</t>
   </si>
   <si>
     <t xml:space="preserve">2884</t>
@@ -296,7 +296,7 @@
     <t xml:space="preserve">672,000</t>
   </si>
   <si>
-    <t xml:space="preserve">2.56%</t>
+    <t xml:space="preserve">2.55%</t>
   </si>
   <si>
     <t xml:space="preserve">6274</t>
@@ -332,7 +332,7 @@
     <t xml:space="preserve">301,000</t>
   </si>
   <si>
-    <t xml:space="preserve">1.94%</t>
+    <t xml:space="preserve">1.91%</t>
   </si>
   <si>
     <t xml:space="preserve">3583</t>
@@ -353,10 +353,22 @@
     <t xml:space="preserve">嘉澤</t>
   </si>
   <si>
-    <t xml:space="preserve">143,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.17%</t>
+    <t xml:space="preserve">159,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.38%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1560</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中砂</t>
+  </si>
+  <si>
+    <t xml:space="preserve">593,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.19%</t>
   </si>
   <si>
     <t xml:space="preserve">6223</t>
@@ -365,22 +377,22 @@
     <t xml:space="preserve">旺矽</t>
   </si>
   <si>
-    <t xml:space="preserve">130,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.95%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1560</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中砂</t>
-  </si>
-  <si>
-    <t xml:space="preserve">456,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.91%</t>
+    <t xml:space="preserve">157,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.13%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">亞翔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">486,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.00%</t>
   </si>
   <si>
     <t xml:space="preserve">3131</t>
@@ -392,7 +404,7 @@
     <t xml:space="preserve">102,000</t>
   </si>
   <si>
-    <t xml:space="preserve">0.90%</t>
+    <t xml:space="preserve">0.88%</t>
   </si>
   <si>
     <t xml:space="preserve">2481</t>
@@ -404,7 +416,7 @@
     <t xml:space="preserve">2,175,000</t>
   </si>
   <si>
-    <t xml:space="preserve">0.81%</t>
+    <t xml:space="preserve">0.80%</t>
   </si>
   <si>
     <t xml:space="preserve">4966</t>
@@ -416,16 +428,7 @@
     <t xml:space="preserve">161,000</t>
   </si>
   <si>
-    <t xml:space="preserve">0.80%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">亞翔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">396,000</t>
+    <t xml:space="preserve">0.77%</t>
   </si>
   <si>
     <t xml:space="preserve">2382</t>
@@ -461,7 +464,7 @@
     <t xml:space="preserve">777,000</t>
   </si>
   <si>
-    <t xml:space="preserve">0.63%</t>
+    <t xml:space="preserve">0.62%</t>
   </si>
   <si>
     <t xml:space="preserve">4770</t>
@@ -494,6 +497,9 @@
     <t xml:space="preserve">67,000</t>
   </si>
   <si>
+    <t xml:space="preserve">0.45%</t>
+  </si>
+  <si>
     <t xml:space="preserve">6143</t>
   </si>
   <si>
@@ -527,7 +533,7 @@
     <t xml:space="preserve">229,000</t>
   </si>
   <si>
-    <t xml:space="preserve">0.31%</t>
+    <t xml:space="preserve">0.30%</t>
   </si>
   <si>
     <t xml:space="preserve">1210</t>
@@ -573,9 +579,6 @@
   </si>
   <si>
     <t xml:space="preserve">191,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.19%</t>
   </si>
   <si>
     <t xml:space="preserve">5347</t>
@@ -1467,7 +1470,7 @@
   <sheetFormatPr defaultColWidth="8.43" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.25" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12.9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10.35" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -1996,343 +1999,343 @@
         <v>137</v>
       </c>
       <c r="D47" s="138" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="139" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B48" s="140" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C48" s="141" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D48" s="142" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="143" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B49" s="144" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C49" s="145" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D49" s="146" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="147" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B50" s="148" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C50" s="149" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D50" s="150" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="151" t="s">
+        <v>151</v>
+      </c>
+      <c r="B51" s="152" t="s">
+        <v>152</v>
+      </c>
+      <c r="C51" s="153" t="s">
+        <v>153</v>
+      </c>
+      <c r="D51" s="154" t="s">
         <v>150</v>
-      </c>
-      <c r="B51" s="152" t="s">
-        <v>151</v>
-      </c>
-      <c r="C51" s="153" t="s">
-        <v>152</v>
-      </c>
-      <c r="D51" s="154" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="155" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B52" s="156" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C52" s="157" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D52" s="158" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="159" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B53" s="160" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C53" s="161" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D53" s="162" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="163" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B54" s="164" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C54" s="165" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D54" s="166" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="167" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B55" s="168" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C55" s="169" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D55" s="170" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="171" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B56" s="172" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C56" s="173" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D56" s="174" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="175" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B57" s="176" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C57" s="177" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D57" s="178" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="179" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B58" s="180" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C58" s="181" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D58" s="182" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="183" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B59" s="184" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C59" s="185" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D59" s="186" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="187" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B60" s="188" t="s">
+        <v>187</v>
+      </c>
+      <c r="C60" s="189" t="s">
+        <v>188</v>
+      </c>
+      <c r="D60" s="190" t="s">
         <v>185</v>
-      </c>
-      <c r="C60" s="189" t="s">
-        <v>186</v>
-      </c>
-      <c r="D60" s="190" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="191" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B61" s="192" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C61" s="193" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D61" s="194" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="195" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B62" s="196" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C62" s="197" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D62" s="198" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="199" t="s">
+        <v>197</v>
+      </c>
+      <c r="B63" s="200" t="s">
+        <v>198</v>
+      </c>
+      <c r="C63" s="201" t="s">
+        <v>199</v>
+      </c>
+      <c r="D63" s="202" t="s">
         <v>196</v>
-      </c>
-      <c r="B63" s="200" t="s">
-        <v>197</v>
-      </c>
-      <c r="C63" s="201" t="s">
-        <v>198</v>
-      </c>
-      <c r="D63" s="202" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="203" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B64" s="204" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C64" s="205" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D64" s="206" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="207" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B65" s="208" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C65" s="209" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D65" s="210" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="211" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B66" s="212" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C66" s="213" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D66" s="214" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="215" t="s">
+        <v>211</v>
+      </c>
+      <c r="B67" s="216" t="s">
+        <v>212</v>
+      </c>
+      <c r="C67" s="217" t="s">
+        <v>206</v>
+      </c>
+      <c r="D67" s="218" t="s">
         <v>210</v>
-      </c>
-      <c r="B67" s="216" t="s">
-        <v>211</v>
-      </c>
-      <c r="C67" s="217" t="s">
-        <v>205</v>
-      </c>
-      <c r="D67" s="218" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="219" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B68" s="220" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C68" s="221" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D68" s="222" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="223" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B69" s="224" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C69" s="225" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D69" s="226" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="227" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B70" s="228" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C70" s="229" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D70" s="230" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="231" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B71" s="232" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C71" s="233" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D71" s="234" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>